<commit_message>
Built Longevity Bonus pay scripts Modified header row of Longevity lookup table
</commit_message>
<xml_diff>
--- a/LookupData/TableLongevity.xlsx
+++ b/LookupData/TableLongevity.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA_Source\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d66x816\Documents\emr_v2_git\LookupData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10560" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10560" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" calcOnSave="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,16 +26,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>YearsOfService</t>
+    <t>Longevity_Percent</t>
   </si>
   <si>
-    <t>PercentToBase</t>
+    <t>Years_Of_Service</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -355,11 +355,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -370,10 +370,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>